<commit_message>
chore: limpeza do repositorio e adicao de arquivos uteis
- Remove 42 scripts temporarios/debug (check_*, fix_*, test_*, find_*, etc.)
- Remove tools/debug/ inteiro (22 scripts de diagnostico one-off)
- Remove snapshots HTML, CSVs do GSC, backups PHP
- Adiciona docs/bling-openapi.json (referencia API Bling v3)
- Adiciona tools/ uteis (oauth_helper, list_lojas, sync_dashboard, vincular)
- Adiciona metricas/ (implementacao analytics, boas praticas)
- Adiciona analytics_unified.php e performance_enhanced.php (tema ativo)
- Adiciona .aiignore, opencode.json, WOOCOMMERCE.xlsx, relatorio analytics
</commit_message>
<xml_diff>
--- a/MIGRAÇÃO/produtos_importacao_bling.xlsx
+++ b/MIGRAÇÃO/produtos_importacao_bling.xlsx
@@ -736,7 +736,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>AVA-COS-ROUPAS</t>
+          <t>AVA-HIG-AGUALAVA</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -941,7 +941,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>CEN-SUP-AMINNU</t>
+          <t>CEN-SUP-AMINNUXI</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1138,7 +1138,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>XTR-SUP-BIOXTR</t>
+          <t>XTR-SUP-BIOSH240</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1343,7 +1343,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>CEN-SUP-COLLCR</t>
+          <t>CEN-FIT-CREAT500</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1538,7 +1538,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>OCE-VIT-CURCUM</t>
+          <t>OCE-NAT-CURCU60</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1743,7 +1743,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>AVA-OIL-ALECRI</t>
+          <t>AVA-OLE-ALECCAPI</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>OCE-SUP-PROVEG</t>
+          <t>OCE-ALI-PROVEG30</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -2141,7 +2141,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>OCE-VIT-FENOGR</t>
+          <t>OCE-NAT-FENOG60</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -2346,7 +2346,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>CEN-SUP-GUARDN</t>
+          <t>CEN-SUP-GUARD30</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -2549,7 +2549,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>AVA-OIL-CHAVER</t>
+          <t>AVA-CHA-CHAVERDE</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -2754,7 +2754,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>AVA-COS-MINIKI</t>
+          <t>AVA-BEB-MINIGIGI</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -2945,7 +2945,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>OCE-VIT-MAGNES</t>
+          <t>OCE-VIT-MAGNE900</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -3150,7 +3150,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>MAH-FOO-COFFEE</t>
+          <t>MAH-ALI-COFFEE22</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -3341,7 +3341,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>CEN-SUP-ARTICU</t>
+          <t>CEN-SUP-ARTIC90</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -3546,7 +3546,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>CEN-OIL-DEALHO</t>
+          <t>CEN-OLE-ALHO500</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -3751,7 +3751,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>AVA-COS-MARACU</t>
+          <t>AVA-COS-MARAC300</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -3956,7 +3956,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>OCE-VIT-OMEGA3</t>
+          <t>OCE-OLE-OMEGA3DH</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -4161,7 +4161,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>AVA-OIL-LAVAND</t>
+          <t>AVA-HIG-PERFU500</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -4366,7 +4366,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>AVA-OIL-PERINT</t>
+          <t>AVA-HIG-PERFU200</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -4557,7 +4557,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>CEN-VIT-RESTOR</t>
+          <t>CEN-VIT-VITLIPO1</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -4764,7 +4764,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>CEN-SUP-ENERGY</t>
+          <t>CEN-FIT-ENERGYATP</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -4969,7 +4969,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>OCE-VIT-ASTAXA</t>
+          <t>OCE-COS-ASTAX405</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -5174,7 +5174,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>MAH-FOO-LEITEP</t>
+          <t>MAH-ALI-LEITE600</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -5379,7 +5379,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>AVA-OIL-APOGEU</t>
+          <t>AVA-OLE-APOGEU42</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -5584,7 +5584,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>BRA-FOO-CHAGEL</t>
+          <t>BRA-CHA-CHAGEL26</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -5777,7 +5777,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>AVA-OIL-ESSENC</t>
+          <t>AVA-OLE-ESSEN30M</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -5974,7 +5974,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>AVA-COS-AGUAPE</t>
+          <t>AVA-HIG-AGUAR110</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -6181,7 +6181,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>MIY-SUP-PROPOL</t>
+          <t>MIY-NAT-PROPOLIS</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -6386,7 +6386,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>MIY-SUP-COLCAI</t>
+          <t>MIY-COS-COLACX10</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -6591,7 +6591,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>MIY-SUP-COLAGE</t>
+          <t>MIY-COS-COLA6000</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -6796,7 +6796,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>MUS-FOO-MUSHIN</t>
+          <t>MUS-ALI-MUSH220G</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -6995,7 +6995,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>BRA-FOO-CAPLIM</t>
+          <t>BRA-CHA-CAPLIM</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -7188,7 +7188,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>BRA-FOO-VERMEL</t>
+          <t>BRA-CHA-FRUTVERM</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -7381,7 +7381,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>BRA-FOO-HIBPES</t>
+          <t>BRA-CHA-HISC PESS</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -7574,7 +7574,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>BRA-FOO-MATLIM</t>
+          <t>BRA-CHA-MATLIMAO</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -7767,7 +7767,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>BRA-FOO-VERTAN</t>
+          <t>BRA-CHA-VERDTANG</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -7960,7 +7960,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>OCE-SUP-BAUNIL</t>
+          <t>OCE-ALI-PROBAUN</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -8167,7 +8167,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>OCE-SUP-CHOCOL</t>
+          <t>OCE-ALI-PROCHOC</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -8374,7 +8374,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>AVA-COS-ESFOLI</t>
+          <t>AVA-COS-ESFOAVAC</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -8579,7 +8579,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>AVA-OIL-ALECR2</t>
+          <t>AVA-OLE-ALE30ML</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -8784,7 +8784,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>AVA-OIL-BAMBU</t>
+          <t>AVA-OLE-BAM30ML</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -8989,7 +8989,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>AVA-OIL-CASCAS</t>
+          <t>AVA-OLE-CAS30ML</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -9194,7 +9194,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>AVA-COS-MINIGI</t>
+          <t>AVA-COS-KITGIGI</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -9399,7 +9399,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>AVA-COS-GIILAZ</t>
+          <t>AVA-COS-GIGILAZ</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -9604,7 +9604,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>MAH-FOO-CACSEL</t>
+          <t>MAH-ALI-CACAU220</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -9809,7 +9809,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>MAH-FOO-ORIGIN</t>
+          <t>MAH-ALI-ORIG220</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -10014,7 +10014,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>OCE-VIT-MAGNE2</t>
+          <t>OCE-VIT-MAG90CAP</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -10221,7 +10221,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>OCE-SUP-PRETRE</t>
+          <t>OCE-FIT-PRE120CP</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -10426,7 +10426,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>MAH-FOO-SUPERF</t>
+          <t>MAH-ALI-SUP840G</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -10627,7 +10627,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>OCE-SUP-VEGETA</t>
+          <t>OCE-ALI-PROT450G</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -10828,7 +10828,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>AVA-COS-LAVAMB</t>
+          <t>AVA-HIG-LAVAMB35</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -11035,7 +11035,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>MAH-FOO-SUPER2</t>
+          <t>MAH-ALI-SUP360G</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -11236,7 +11236,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>XTR-SUP-NITRAT</t>
+          <t>XTR-FIT-NIT300G</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -11441,7 +11441,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>AVA-COS-APOGEU</t>
+          <t>AVA-COS-APOG190G</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -11652,7 +11652,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>XTR-SUP-BETLIM</t>
+          <t>XTR-FIT-BETLIMAO</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -11859,7 +11859,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>AVA-COS-SABLIQ</t>
+          <t>AVA-HIG-LIQ400ML</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -12060,7 +12060,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>MUS-FOO-AVECOG</t>
+          <t>MUS-ALI-AVEIA40G</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -12267,7 +12267,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>AVA-COS-CHAVER</t>
+          <t>AVA-HIG-CHAVERDE</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -12474,7 +12474,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>AVA-COS-APOGE2</t>
+          <t>AVA-HIG-APOG500M</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -12681,7 +12681,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>OCE-SUP-MATLIO</t>
+          <t>OCE-ALI-LIMAO150</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -12888,7 +12888,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>OCE-SUP-SLIMBO</t>
+          <t>OCE-SUP-SLIM60CP</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -13095,7 +13095,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>OCE-SUP-SPIRUL</t>
+          <t>OCE-SUP-SPIR120C</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -13302,7 +13302,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>OCE-FOO-PROTEI</t>
+          <t>OCE-ALI-PROVEGB</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -13507,7 +13507,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>OCE-FOO-PROTE2</t>
+          <t>OCE-ALI-PROVECH</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -13712,7 +13712,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>AVA-COS-SABONE</t>
+          <t>AVA-HIG-SABALE40</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -13919,7 +13919,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>AVA-COS-SABON2</t>
+          <t>AVA-HIG-SABFLOAL</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -14126,7 +14126,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>MAH-FOO-SUPER3</t>
+          <t>MAH-ALI-ACACAM36</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -14321,7 +14321,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>MAH-FOO-SUPER4</t>
+          <t>MAH-ALI-CACCCU36</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -14528,7 +14528,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>MAH-FOO-SUPER5</t>
+          <t>MAH-ALI-ACACAM84</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -14723,7 +14723,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>MAH-FOO-SUPER6</t>
+          <t>MAH-ALI-CACCCU84</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -14930,7 +14930,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>CEN-VIT-BCOMPL</t>
+          <t>CEN-VIT-BCOMP120</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -15137,7 +15137,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>CEN-SUP-BOMCIC</t>
+          <t>CEN-SUP-BOMCIC60</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -15344,7 +15344,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>HER-COS-DESODO</t>
+          <t>HER-COS-ROLLROS</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -15551,7 +15551,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>XTR-SUP-DISPLA</t>
+          <t>XTR-FIT-PRE90G</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -15744,7 +15744,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>XTR-SUP-INTRAT</t>
+          <t>XTR-FIT-INTTRASAC</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -15947,7 +15947,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>MUS-FOO-LATTEC</t>
+          <t>MUS-ALI-LATCOFFE</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -16152,7 +16152,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>CEN-SUP-LEVSEN</t>
+          <t>CEN-ALI-LEVMACA</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -16359,7 +16359,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>EMP-FOO-FLORES</t>
+          <t>EMP-ALI-MELLARA3</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -16566,7 +16566,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>HER-OIL-ROSA</t>
+          <t>HER-OLE-ROSMOS10</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -16773,7 +16773,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>HER-OIL-SEMENT</t>
+          <t>HER-OLE-SEMEUVA</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -16980,7 +16980,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>CEN-SUP-PILLFO</t>
+          <t>CEN-SUP-PILL60</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -17187,7 +17187,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>CEN-SUP-POLIOM</t>
+          <t>CEN-SUP-POLIOMEG</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -17394,7 +17394,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>CEN-SUP-MAGNES</t>
+          <t>CEN-SUP-POOLMAG9</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -17601,7 +17601,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>CEN-SUP-AMINN2</t>
+          <t>CEN-SUP-AMILIVRE</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -17794,7 +17794,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>HER-COS-SERUMF</t>
+          <t>HER-COS-SERUFACI</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -18005,7 +18005,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>MIV-SUP-SHAKEP</t>
+          <t>MIV-FIT-POS</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -18210,7 +18210,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>MIV-SUP-SHAKE2</t>
+          <t>MIV-FIT-PREACALA</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -18415,7 +18415,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>MIV-SUP-SHAKED</t>
+          <t>MIV-FIT-SHAKMAT</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -18618,7 +18618,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>CEN-VIT-VITAMI</t>
+          <t>CEN-VIT-VITD3200</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -18825,7 +18825,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>OCE-FOO-PROTE3</t>
+          <t>OCE-ALI-DUOPROVE</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -19030,7 +19030,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>CEN-FOO-LIMAO</t>
+          <t>CEN-ALI-LIMAO</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -19235,7 +19235,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>CEN-FOO-TANGE</t>
+          <t>CEN-ALI-TANGERIN</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -19440,7 +19440,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>CEN-FOO-SEM</t>
+          <t>CEN-ALI-SEMSABOR</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -19645,7 +19645,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>CEN-SUP-ENERG2</t>
+          <t>CEN-FIT-ATPLIMAO</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -19850,7 +19850,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>CEN-SUP-ENERG3</t>
+          <t>CEN-FIT-ATP10G</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -20043,7 +20043,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>MUS-FOO-CHAI</t>
+          <t>MUS-CHA-MUSHCHAI</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -20248,7 +20248,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>CEN-SUP-CREATI</t>
+          <t>CEN-SUP-CREA500G</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -20449,7 +20449,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>CEN-SUP-CREAT2</t>
+          <t>CEN-SUP-CREALM500</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -20654,7 +20654,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>AVA-COS-ROUPA2</t>
+          <t>AVA-COS-FLOR1100</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -20861,7 +20861,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>AVA-COS-ROUPA3</t>
+          <t>AVA-COS-ALEC1100</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -21068,7 +21068,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>CEN-FOO-LIMAO2</t>
+          <t>CEN-ALI-LIMAO2</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -21267,7 +21267,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>CEN-FOO-SEM2</t>
+          <t>CEN-ALI-SEMSA2</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -21468,7 +21468,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>CEN-SUP-ENERG4</t>
+          <t>CEN-FIT-ATPTANGE</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -21673,7 +21673,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>EDI-MED-DICION</t>
+          <t>EDI-NAT-DICIONAR</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -21865,7 +21865,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>SOL-COS-CONDI</t>
+          <t>SOL-COS-CONDIBAR</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -22050,7 +22050,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>SOL-COS-SHAMPO</t>
+          <t>SOL-COS-SHACAI</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -22237,7 +22237,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>SOL-COS-SABONE</t>
+          <t>SOL-HIG-DETOX</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -22422,7 +22422,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>SOL-COS-LATINH</t>
+          <t>SOL-ALI-LATPRATA</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -22609,7 +22609,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>SOL-OIL-FACIAL</t>
+          <t>SOL-OLE-FACIAL</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -22796,7 +22796,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>SOL-COS-SHAMP2</t>
+          <t>SOL-COS-SHACA2</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -22993,7 +22993,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>SOL-OIL-FACIA2</t>
+          <t>SOL-OLE-FACIA2</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -23192,7 +23192,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>XTR-SUP-INTRA</t>
+          <t>XTR-FIT-PRE1KG</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -23375,7 +23375,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>XTR-SUP-H2GEL</t>
+          <t>XTR-FIT-H2GEL75</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -23570,7 +23570,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>MUS-FOO-BAR</t>
+          <t>MUS-ALI-VANI45</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -23765,7 +23765,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>MUS-FOO-BAR2</t>
+          <t>MUS-ALI-VANI45CX</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -23958,7 +23958,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>LAS-OIL-ALECRI</t>
+          <t>LAS-OLE-ALECQT</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -24141,7 +24141,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>LAS-OIL-CAPIM</t>
+          <t>LAS-OLE-CAPIM10</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -24322,7 +24322,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>LAS-OIL-ALECR2</t>
+          <t>LAS-OLE-ALEC10</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -24505,7 +24505,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>LAS-OIL-CAPIM2</t>
+          <t>LAS-OLE-CAPIM2</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -24686,7 +24686,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>LAS-COS-SERUM</t>
+          <t>LAS-COS-CLEO30</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -24869,7 +24869,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>LAS-OIL-EUCA85</t>
+          <t>LAS-OLE-EUCA10</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -25050,7 +25050,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>LAS-OIL-HORTEL</t>
+          <t>LAS-OLE-HORT10</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -25231,7 +25231,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>LAS-OIL-EUCA82</t>
+          <t>LAS-OLE-EUCA12</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -25412,7 +25412,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>LAS-COS-CLEOPA</t>
+          <t>LAS-COS-CLEO32</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -25595,7 +25595,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>LAS-OIL-CAPLIMA</t>
+          <t>LAS-OLE-CAPIM3</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -25776,7 +25776,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>LAS-OIL-ALECR3</t>
+          <t>LAS-OLE-ALEC12</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -25959,7 +25959,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>LAS-OIL-ALECR4</t>
+          <t>LAS-OLE-ALEC13</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -26142,7 +26142,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>LAS-OIL-LAVFIN</t>
+          <t>LAS-OLE-LAVA10</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -26325,7 +26325,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>LAS-OIL-LAVFI2</t>
+          <t>LAS-OLE-LAVA12</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -26506,7 +26506,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>LAS-OIL-TEATRE</t>
+          <t>LAS-OLE-TEAT10</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -26689,7 +26689,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>LAS-OIL-SANGDE</t>
+          <t>LAS-OLE-SANG10</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -26870,7 +26870,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>LAS-OIL-BERGAM</t>
+          <t>LAS-OLE-BERG10</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -27053,7 +27053,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>LAS-OIL-ALECR5</t>
+          <t>LAS-OLE-ALEC14</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -27234,7 +27234,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>LAS-OIL-CAPLI2</t>
+          <t>LAS-OLE-CAPIM4</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -27417,7 +27417,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>LAS-OIL-EUCA83</t>
+          <t>LAS-OLE-EUCA13</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -27598,7 +27598,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>LAS-OIL-HORTE2</t>
+          <t>LAS-OLE-HORT12</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -27779,7 +27779,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>LAS-OIL-LAVFI3</t>
+          <t>LAS-OLE-LAVA13</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -27960,7 +27960,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>LAS-OIL-TEATR2</t>
+          <t>LAS-OLE-TEAT12</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -28141,7 +28141,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>LAS-OIL-LAVFI4</t>
+          <t>LAS-OLE-LAVA14</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -28324,7 +28324,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>LAS-OIL-SANGD2</t>
+          <t>LAS-OLE-SANG12</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
@@ -28505,7 +28505,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>LAS-OIL-BERGA2</t>
+          <t>LAS-OLE-BERG12</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -28688,7 +28688,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>LAS-OIL-BERGA3</t>
+          <t>LAS-OLE-BERG13</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -28871,7 +28871,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>LAS-OIL-ALECR6</t>
+          <t>LAS-OLE-ALEC15</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -29054,7 +29054,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>GRA-COS-SABGLI</t>
+          <t>GRA-HIG-SABGLAV</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -29237,7 +29237,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>GRA-COS-REFSAB</t>
+          <t>GRA-HIG-REFCALE</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -29420,7 +29420,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>GRA-COS-COLBEB</t>
+          <t>GRA-BEB-COLERV</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -29601,7 +29601,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>PHE-COS-SABBOU</t>
+          <t>PHE-HIG-SABGERA</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -29784,7 +29784,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>PHE-COS-COLBOU</t>
+          <t>PHE-COS-COLGERA</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
@@ -29967,7 +29967,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>GRA-COS-SABGL2</t>
+          <t>GRA-BEB-SABGCAMO</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
@@ -30152,7 +30152,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>MAH-FOO-CACSE2</t>
+          <t>MAH-ALI-CACAUSEL</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
@@ -30333,7 +30333,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>AMO-COS-ESFOLI</t>
+          <t>AMO-COS-ESFOLMUL</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
@@ -30516,7 +30516,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>AMO-COS-BATOMC</t>
+          <t>AMO-COS-BATOCREMP</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
@@ -30697,7 +30697,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>AMO-COS-BATOMS</t>
+          <t>AMO-COS-BATSOLMOR</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
@@ -30878,7 +30878,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>AMO-COS-BALMLB</t>
+          <t>AMO-COS-BALMLAB</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
@@ -31061,7 +31061,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>AMO-COS-LIPTIN</t>
+          <t>AMO-COS-LIPTAMORA</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -31242,7 +31242,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>AMO-COS-BALSAM</t>
+          <t>AMO-COS-BALSDEMAQ</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -31425,7 +31425,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>AMO-COS-MASCAR</t>
+          <t>AMO-COS-MASCCILPR</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
@@ -31608,7 +31608,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>AMO-COS-DELINE</t>
+          <t>AMO-COS-DELOLHPR</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
@@ -31791,7 +31791,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>AMO-COS-SABONL</t>
+          <t>AMO-HIG-SABLIQPI</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
@@ -31972,7 +31972,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>AMO-COS-SUPORT</t>
+          <t>AMO-COS-SUPMAQSO</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
@@ -32155,7 +32155,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>AMO-COS-BATOMG</t>
+          <t>AMO-COS-BATSOLGO</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
@@ -32336,7 +32336,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>MUS-FOO-MUSHBA</t>
+          <t>MUS-ALI-MUSHMO</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
@@ -32521,7 +32521,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>MUS-FOO-FANTAO</t>
+          <t>MUS-ALI-FANTOAT</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
@@ -32712,7 +32712,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>MUS-FOO-MUSHBC</t>
+          <t>MUS-ALI-MUSHMO12</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
@@ -32895,7 +32895,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>PHE-COS-CAIXAS</t>
+          <t>PHE-HIG-SABVINHO</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
@@ -33082,7 +33082,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>PHE-COS-COLONI</t>
+          <t>PHE-COS-COLGER20</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
@@ -33267,7 +33267,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>PHE-COS-SABROS</t>
+          <t>PHE-HIG-SABROS90</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
@@ -33452,7 +33452,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>CEN-SUP-GUARDI</t>
+          <t>CEN-SUP-GUARCENT</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
@@ -33639,7 +33639,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>AMO-COS-BASESO</t>
+          <t>AMO-COS-BASESOL</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
@@ -33820,7 +33820,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>GRA-COS-SHAMPO</t>
+          <t>GRA-HIG-SHAMPPET</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
@@ -33995,7 +33995,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>GRA-COS-VELAPE</t>
+          <t>GRA-COS-VELAPERF</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
@@ -34168,7 +34168,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>GRA-COS-COLBE2</t>
+          <t>GRA-BEB-COLBEBE</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
@@ -34343,7 +34343,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>LAS-OIL-MANTEI</t>
+          <t>LAS-COS-MANTEVEG</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
@@ -34520,7 +34520,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>LAS-OIL-HIDROL</t>
+          <t>LAS-COS-HIDROLAT</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
@@ -34693,7 +34693,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>NOV-SUP-JAPECN</t>
+          <t>NOV-CHA-JAPEC100</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
@@ -34874,7 +34874,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>NOV-SUP-TILIAF</t>
+          <t>NOV-CHA-TILIA100</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
@@ -35055,7 +35055,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>NOV-SUP-ASSAPE</t>
+          <t>NOV-CHA-ASSAP100</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
@@ -35236,7 +35236,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>NOV-SUP-QUEBRA</t>
+          <t>NOV-CHA-QUEBR100</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
@@ -35417,7 +35417,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>NOV-SUP-PIMMAC</t>
+          <t>NOV-CHA-PIMEN100</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
@@ -35598,7 +35598,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>NOV-SUP-ALCACH</t>
+          <t>NOV-CHA-ALCAC100</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
@@ -35779,7 +35779,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>NOV-SUP-JALAPA</t>
+          <t>NOV-CHA-JALAPA</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
@@ -35960,7 +35960,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>NOV-SUP-IPEROX</t>
+          <t>NOV-CHA-IPEROXO</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
@@ -36143,7 +36143,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>NOV-SUP-MACAEL</t>
+          <t>NOV-CHA-MACAELEF</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
@@ -36326,7 +36326,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>NOV-SUP-RUIBAR</t>
+          <t>NOV-CHA-RUIBARBO</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
@@ -36509,7 +36509,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>NOV-SUP-NOCACH</t>
+          <t>NOV-CHA-NOCACHOR</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
@@ -36692,7 +36692,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>NOV-SUP-GENGIB</t>
+          <t>NOV-CHA-GENGIBRE</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
@@ -36875,7 +36875,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>NOV-FOO-JATOBA</t>
+          <t>NOV-ALI-JATOBA</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
@@ -37058,7 +37058,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>NOV-SUP-PARATU</t>
+          <t>NOV-NAT-PARATUDO</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
@@ -37243,7 +37243,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>NOV-FOO-QUINOA</t>
+          <t>NOV-ALI-QUINOA</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
@@ -37428,7 +37428,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>MAH-SUP-SUPERF</t>
+          <t>MAH-ALI-ACAI</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
@@ -37609,7 +37609,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>AMO-COS-ILUMIN</t>
+          <t>AMO-COS-ILUMINPO</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
@@ -37794,7 +37794,7 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>LAS-COS-KARITE</t>
+          <t>LAS-COS-KARITE10</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
@@ -37979,7 +37979,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>XTR-SUP-INTRA2</t>
+          <t>XTR-FIT-INTRA1KG</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
@@ -38162,7 +38162,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>NOV-SUP-GUARAN</t>
+          <t>NOV-CHA-GUARANA</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
@@ -38349,7 +38349,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>LAS-OIL-INSPIR</t>
+          <t>LAS-OLE-INSPIR5</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
@@ -38534,7 +38534,7 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>MOI-FOO-STROOP</t>
+          <t>MOI-ALI-STROOP</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
@@ -38721,7 +38721,7 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>GRA-COS-LIMAOS</t>
+          <t>GRA-HIG-LIMAOSIC</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
@@ -38904,7 +38904,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>PHE-COS-LIMAOS</t>
+          <t>PHE-COS-LIM200</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
@@ -39089,7 +39089,7 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>GRA-COS-CALEND</t>
+          <t>GRA-HIG-CALEN300</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
@@ -39272,7 +39272,7 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>AMO-COS-TONAKA</t>
+          <t>AMO-COS-TONAK15</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
@@ -39457,7 +39457,7 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>AMO-COS-TONAK2</t>
+          <t>AMO-COS-TONAK05</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
@@ -39642,7 +39642,7 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>AMO-COS-TONAK3</t>
+          <t>AMO-COS-TONAK10</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
@@ -39827,7 +39827,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>AMO-COS-TONAK4</t>
+          <t>AMO-COS-TONAK20</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
@@ -40012,7 +40012,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>AMO-COS-TONAK5</t>
+          <t>AMO-COS-TONAK25</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
@@ -40197,7 +40197,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>AMO-COS-TONAK6</t>
+          <t>AMO-COS-TONAK30</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
@@ -40382,7 +40382,7 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>AMO-COS-TONAK7</t>
+          <t>AMO-COS-TONAK40</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
@@ -40567,7 +40567,7 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>AMO-COS-TONAK8</t>
+          <t>AMO-COS-TONAK42</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
@@ -40752,7 +40752,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>AMO-COS-TONAK9</t>
+          <t>AMO-COS-TONAK45</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
@@ -40937,7 +40937,7 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>AMO-COS-TONAK10</t>
+          <t>AMO-COS-TONAK50</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
@@ -41122,7 +41122,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>AMO-COS-TONAK11</t>
+          <t>AMO-COS-TONAK55</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
@@ -41307,7 +41307,7 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>AMO-COS-AK60</t>
+          <t>AMO-COS-TON60</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
@@ -41492,7 +41492,7 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>AMO-COS-AK70</t>
+          <t>AMO-COS-TON70</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
@@ -41677,7 +41677,7 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>AMO-COS-AK80</t>
+          <t>AMO-COS-TON80</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
@@ -41862,7 +41862,7 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>CEN-SUP-GUARD</t>
+          <t>CEN-VIT-GUARDSS</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
@@ -42047,7 +42047,7 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>CEN-SUP-GUARD2</t>
+          <t>CEN-VIT-GUARDL</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
@@ -42234,7 +42234,7 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>GRA-COS-SUAVE</t>
+          <t>GRA-BEB-SUAVE</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
@@ -42411,7 +42411,7 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>GRA-COS-NEUTRO</t>
+          <t>GRA-BEB-NEUTRO</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
@@ -42588,7 +42588,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>GRA-COS-DESEMB</t>
+          <t>GRA-BEB-DESEMB</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
@@ -42765,7 +42765,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>GRA-COS-ERVA</t>
+          <t>GRA-BEB-ERVADOC</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
@@ -42942,7 +42942,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>GRA-COS-CHABRA</t>
+          <t>GRA-COS-CHABRAN</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
@@ -43119,7 +43119,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>LAS-OIL-ALECR7</t>
+          <t>LAS-OLE-ALECRIM</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
@@ -43296,7 +43296,7 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>LAS-OIL-KARITE</t>
+          <t>LAS-OLE-KARITE</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
@@ -43475,7 +43475,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>LAS-OIL-MANGA</t>
+          <t>LAS-OLE-MANGA</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
@@ -43654,7 +43654,7 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>CEN-FOO-LIMAO3</t>
+          <t>CEN-FIT-LIMAO</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
@@ -43851,7 +43851,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>CEN-FOO-TANGE2</t>
+          <t>CEN-FIT-TANGER</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
@@ -44048,7 +44048,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>CEN-FOO-LIMAO4</t>
+          <t>CEN-ALI-LIMAO3</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
@@ -44245,7 +44245,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>CEN-FOO-TANGE3</t>
+          <t>CEN-ALI-TANGER</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
@@ -44442,7 +44442,7 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>CEN-FOO-TANGE4</t>
+          <t>CEN-ALI-TANGE2</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
@@ -44643,7 +44643,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>MUS-FOO-FRUTAS</t>
+          <t>MUS-ALI-FRUTVER</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
@@ -44838,7 +44838,7 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>MUS-FOO-CARAME</t>
+          <t>MUS-ALI-CARAMELO</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
@@ -45033,7 +45033,7 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>XTR-FOO-ABACAX</t>
+          <t>XTR-CHA-ABACHOR</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
@@ -45240,7 +45240,7 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>XTR-FOO-BETERR</t>
+          <t>XTR-CHA-BETLIMG</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
@@ -45447,7 +45447,7 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>XTR-FOO-BETER2</t>
+          <t>XTR-CHA-BETLI2</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
@@ -45644,7 +45644,7 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>XTR-FOO-MATEVE</t>
+          <t>XTR-CHA-MATEVER</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
@@ -45841,7 +45841,7 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>XTR-FOO-ABACA2</t>
+          <t>XTR-CHA-ABACH2</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">

</xml_diff>